<commit_message>
Fix: duplicates date,name broke pivot script
</commit_message>
<xml_diff>
--- a/sylvanator.xlsx
+++ b/sylvanator.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,187 +441,179 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2021-03-13 Saturday</t>
+          <t>2021-04-02 Friday</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>2021-03-14 Sunday</t>
+          <t>2021-04-03 Saturday</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>2021-03-15 Monday</t>
+          <t>2021-04-04 Sunday</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>2021-03-16 Tuesday</t>
+          <t>2021-04-05 Monday</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Amerix</t>
+          <t>Alukard</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Tanquid Hunxe DIESEL 10 PPM 1400.0 VARO Energy Marketing AG</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ARA MOGAS E5 1000.0 VARO Energy Netherlands B.V.</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Amstel</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>Amerix</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>VARO Geertruidenberg DIESEL B7 1500.0 VARO Energy Marketing AG</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>GPS Amsterdam EURO95 nan VARO Energy Marketing AG</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Arne</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>Amstel</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Oiltanking Amsterdam (OTA) EUROBOB tbv E10 1900.0 Totsa Total Oil Trading SA</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Zeeland Refinery DIESEL 10 PPM 1050.0 Total Belgium NV</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Bergse Diep</t>
+          <t>Arne</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Zeeland Refinery DIESEL 10 PPM 3006.0 Total Belgium NV</t>
+          <t>GPS Amsterdam GASOLINE ETHANOL MIXTURE nan VARO Energy Marketing AG</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Vlissingen DIESEL 10 PPM 3300.0 Total Belgium NV</t>
-        </is>
-      </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Bergse Diep</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Esso Botlek DIESEL 10 PPM 2700.0 Vitol SA</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Vlissingen DIESEL 10 PPM 3300.0 Kuwait Petroleum Nederland BV</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Vlissingen DIESEL 10 PPM 3100.0 LITASCO S.A</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Company</t>
+          <t>Blikplaat</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Total Raffinaderij Antwerpen (TRA) DIESEL/GASOIL 50 PPM UNDYED 1100.0 Total Belgium NV</t>
+          <t>Standic Terminal Dordrecht B100 FAME 1000.0 VARO Energy Marketing AG</t>
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Enviem Nigtevecht DIESEL B7 1200.0 VARO Energy Netherlands B.V.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Connemara</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>DOW Terneuzen TN100 2500.0 VARO Energy Marketing AG</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Enviem Nigtevecht DIESEL B7 2100.0 VARO Energy Marketing AG</t>
-        </is>
-      </c>
+          <t>Chris</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Rotterdam DIESEL 10 PPM 2250.0 POWER TRADE SRO&amp;CO</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Damiano</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Eurotank Terminal Amsterdam (ETA) DIESEL 10 PPM 1100.0 Vitol SA</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Standic Terminal Dordrecht B100 FAME 1000.0 VARO Energy Marketing AG</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>VARO Geertruidenberg DIESEL B7 1500.0 VARO Energy Marketing AG</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Diff</t>
+          <t>Corylophida</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Zeeland Refinery DIESEL 10 PPM 1100.0 Kuwait Petroleum Nederland BV</t>
+          <t>Total Raffinaderij Antwerpen (TRA) DIESEL/GASOIL 50 PPM UNDYED 1500.0 Total Belgium NV</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Vlissingen DIESEL 10 PPM 1100.0 Total Belgium NV</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Eede</t>
+          <t>Damiano</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Shell Pernis GASOIL 0.1 RED DYED nan Shell Trading Rotterdam BV</t>
+          <t>Enviem Nigtevecht DIESEL B7 1450.0 VARO Energy Netherlands B.V.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
@@ -629,270 +621,270 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Eiltank 39</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>GPS Amsterdam SUPERPLUS 98 nan VARO Energy Marketing AG</t>
-        </is>
-      </c>
+          <t>Diff</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Vlissingen DIESEL 10 PPM 1500.0 LITASCO S.A</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Eiltank 69</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+          <t>Eede</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Esso Botlek DIESEL 10 PPM 1720.0 POWER TRADE SRO&amp;CO</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Stargate Rotterdam DIESEL 10 PPM 2040.0 Gunvor SA</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>ARA DIESEL 10 PPM 1720.0 Vitol SA</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Endurance</t>
+          <t>Eiltank 39</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Stargate Rotterdam DIESEL 10 PPM 2250.0 Gunvor SA</t>
+          <t>GPS Amsterdam SUPERPLUS 98 nan VARO Energy Marketing AG</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Eurotank Terminal Amsterdam (ETA) DIESEL 10 PPM 2700.0 Vitol SA</t>
-        </is>
-      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Endurance II</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
+          <t>Eiltank 69</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Esso Antwerpen DIESEL/GASOIL 50 PPM RED DYED 1900.0 Belgomine</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Zeeland Refinery DIESEL 10 PPM 3000.0 Kuwait Petroleum Nederland BV</t>
-        </is>
-      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Fidelity</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr"/>
+          <t>Eiltank 84</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Stargate Rotterdam DIESEL 10 PPM 1500.0 Vitol SA</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Eurotank Terminal Amsterdam (ETA) DIESEL 10 PPM 2400.0 Vitol SA</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Antwerpen DIESEL 10 PPM 1500.0 POWER TRADE SRO&amp;CO</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Endurance</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Oiltanking Amsterdam (OTA) EUROBOB tbv E10 2100.0 Totsa Total Oil Trading SA</t>
-        </is>
-      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>AR (AMS / RTM) DIESEL 10 PPM 2250.0 Vitol SA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Grevelingen</t>
+          <t>Endurance II</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Zeeland Refinery DIESEL 10 PPM 3100.0 Total Belgium NV</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Standic Terminal Dordrecht B100 FAME 2500.0 VARO Energy Marketing AG</t>
+        </is>
+      </c>
       <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Hanneke</t>
+          <t>Fidelity</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Esso Botlek DIESEL 10 PPM 1500.0 POWER TRADE SRO&amp;CO</t>
+          <t>Stargate Rotterdam DIESEL 10 PPM 2400.0 Van Kessel Olie</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Rotterdam DIESEL 10 PPM 1100.0 POWER TRADE SRO&amp;CO</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Rotterdam DIESEL 10 PPM 2400.0 POWER TRADE SRO&amp;CO</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Hartelstroom</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Total Raffinaderij Antwerpen (TRA) EUROBOB tbv E10 2100.0 Total Belgium NV</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>AR (AMS / RTM) EUROBOB tbv E10 nan Phillips 66 Limited</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Julia</t>
+          <t>Gracias</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ARA DIESEL 10 PPM 1700.0 VARO Energy Netherlands B.V.</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>GPS Amsterdam GASOLINE ETHANOL MIXTURE nan VARO Energy Marketing AG</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Markstroom</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Sea Tank Q700B EUROBOB tbv E10 2100.0 LITASCO S.A</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
+          <t>Grevelingen</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Vlissingen DIESEL 10 PPM 3100.0 Total Belgium NV</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Milly</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
+          <t>Hanneke</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Enviem Nigtevecht DIESEL B7 1250.0 VARO Energy Netherlands B.V.</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>VARO Dortmund 2 DIESEL B7 1100.0 VARO Energy Marketing AG</t>
-        </is>
-      </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Nieuwe Maas</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Evos Amsterdam EUROBOB tbv E10 2100.0 BP Oil International LTD</t>
-        </is>
-      </c>
+          <t>Illusion</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Eurotank Terminal Amsterdam (ETA) DIESEL 10 PPM 3100.0 Vitol SA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Rotterdam HYDROTREATED VEGETABLE OIL (HVO) 3000.0 VARO Energy Marketing AG</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Pegasus</t>
+          <t>Julia</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GPS Amsterdam EURO95 nan VARO Energy Marketing AG</t>
+          <t>GPS Amsterdam SUPERPLUS 98 nan VARO Energy Marketing AG</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>GPS Amsterdam EURO95 nan VARO Energy Marketing AG</t>
-        </is>
-      </c>
+      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Poseidon</t>
+          <t>Margret Deymann</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Evos Amsterdam EUROBOB tbv E10 2100.0 BP Oil International LTD</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Rotterdam DIESEL 10 PPM RED DYED 2000.0 Kuwait Petroleum Nederland BV</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Presto</t>
+          <t>Markstroom</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Zeeland Refinery DIESEL 10 PPM 2200.0 LITASCO S.A</t>
+          <t>Antwerpen DIESEL 10 PPM 2250.0 Total Belgium NV</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Vlissingen DIESEL 10 PPM 2500.0 Kuwait Petroleum Nederland BV</t>
-        </is>
-      </c>
+      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Savona</t>
+          <t>Milly</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Stargate Rotterdam DIESEL 10 PPM 2250.0 Gunvor SA</t>
+          <t>Esso Antwerpen DIESEL/GASOIL 50 PPM UNDYED 1100.0 VARO Energy Netherlands B.V.</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
@@ -900,48 +892,48 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Schelde</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
+          <t>Monica</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Sea Tank Q700B DIESEL 10 PPM 2000.0 VARO Energy Netherlands B.V.</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Stargate Rotterdam DIESEL 10 PPM 1500.0 Gunvor SA</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>GPS Amsterdam SUPERPLUS 98 nan VARO Energy Marketing AG</t>
-        </is>
-      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Servio</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr"/>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Vopak Europoort DIESEL 10 PPM 2600.0 POWER TRADE SRO&amp;CO</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Rotterdam DIESEL 10 PPM 2250.0 POWER TRADE SRO&amp;CO</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Somtrans 18</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr"/>
+          <t>Pegasus</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Eurotank Terminal Amsterdam (ETA) EUROBOB tbv E10 nan Phillips 66 Limited</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Eurotank Terminal Amsterdam (ETA) DIESEL 10 PPM 2250.0 Vitol SA</t>
+          <t>GPS Amsterdam SUPERPLUS 98 nan VARO Energy Marketing AG</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
@@ -949,28 +941,32 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Poseidon</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Sea Tank Q700B DIESEL 10 PPM 2650.0 POWER TRADE SRO&amp;CO</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Botlek Tank Terminal EUROBOB tbv E5 1900.0 Vitol SA</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Rotterdam ETBE 2100.0 Lyondell</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Tripolis</t>
+          <t>Presto</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Eurotank Terminal Amsterdam (ETA) DIESEL/GASOIL 50 PPM UNDYED 2000.0 VARO Energy Marketing AG</t>
+          <t>Antwerpen DIESEL/GASOIL 50 PPM RED DYED 2500.0 Total Belgium NV</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
@@ -979,17 +975,96 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
+          <t>Schelde</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>VARO Geertruidenberg SUPERPLUS 98 nan VARO Energy Marketing AG</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Servio</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>VARO Geertruidenberg DIESEL B7 2250.0 VARO Energy Marketing AG</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Rotterdam DIESEL 10 PPM 2250.0 POWER TRADE SRO&amp;CO</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>Somtrans 18</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Standic Terminal Dordrecht B100 FAME 2500.0 VARO Energy Marketing AG</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>Tripolis</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Shell Wesseling DIESEL 10 PPM 2000.0 Shell Trading Rotterdam BV</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>Ulekrite</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Enviem Nigtevecht DIESEL B7 1250.0 VARO Energy Netherlands B.V.</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
           <t>Wiki</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Esso Botlek DIESEL 10 PPM 1200.0 POWER TRADE SRO&amp;CO</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Enviem Nigtevecht DIESEL B7 1200.0 VARO Energy Netherlands B.V.</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>